<commit_message>
updates for MFC July 1 report
</commit_message>
<xml_diff>
--- a/outputs_report/Report_tables_part1(2).xlsx
+++ b/outputs_report/Report_tables_part1(2).xlsx
@@ -3,19 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D27AB9-6BD6-4898-B605-BD7D3A54B33E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094A8ED8-6DB6-4F43-920E-C776BAD727DF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="GDP" sheetId="4" r:id="rId1"/>
-    <sheet name="Stock" sheetId="2" r:id="rId2"/>
-    <sheet name="SimSummary_historical" sheetId="1" r:id="rId3"/>
-    <sheet name="SimulationParms_forward" sheetId="7" r:id="rId4"/>
-    <sheet name="SimulationParms_historical" sheetId="9" r:id="rId5"/>
-    <sheet name="SimulationParms_historical_old" sheetId="3" r:id="rId6"/>
-    <sheet name="Reference assumption" sheetId="6" r:id="rId7"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId8"/>
+    <sheet name="TOC" sheetId="11" r:id="rId1"/>
+    <sheet name="GDP" sheetId="4" r:id="rId2"/>
+    <sheet name="Stock" sheetId="2" r:id="rId3"/>
+    <sheet name="SimSummary_historical" sheetId="1" r:id="rId4"/>
+    <sheet name="SimSummary_historical_short" sheetId="10" r:id="rId5"/>
+    <sheet name="SimulationParms_forward" sheetId="7" r:id="rId6"/>
+    <sheet name="SimulationParms_historical" sheetId="9" r:id="rId7"/>
+    <sheet name="SimulationParms_historical_old" sheetId="3" r:id="rId8"/>
+    <sheet name="Reference assumption" sheetId="6" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId10"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="172">
   <si>
     <t>AR1</t>
   </si>
@@ -487,12 +489,6 @@
     <t>95th percentile</t>
   </si>
   <si>
-    <t>Standard Deveviation</t>
-  </si>
-  <si>
-    <t>Number of recession</t>
-  </si>
-  <si>
     <t>Median</t>
   </si>
   <si>
@@ -538,19 +534,120 @@
   <si>
     <t>Distribution of simulation results
 (2,000 simulations; 63 years in each simulation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes: 
+1. Adjustments are made to the quarterly parameters estimated with historical data to ensure the simulated results for annual data (converted from simulated quarterly data) are consistent with the target assumptions for annual data. The variables that have been adjusted and their historical-data based estimates (all for quarterly data) are expected GDP growth in expansion (0.95%), GDP growth in recession (-0.55%), expected stock return in expansion (3.2%), expected stock return in recession (-1.4%), expected bond return (1.6%), standard deviation of bond return (5.1%). (Historical bond returns are for long-term corporate bond)  
+3. The target annual GDP growth is obtained from the 30-year projection of potential growth GDP made by CBO (2017). The target assumptions on annual stock and bond returns are generally consistent with the capital market assumptions used in Mennis, et. al (2017).  </t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Median of the simulated distribution
+(2,000 simulations)</t>
+  </si>
+  <si>
+    <t>Number of recessions</t>
+  </si>
+  <si>
+    <t>Number of  expansions</t>
+  </si>
+  <si>
+    <t>Summary statistics for historical and simulated data</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kurtosis
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Measure of heavy-tailedness)</t>
+    </r>
+  </si>
+  <si>
+    <t>Economic regimes</t>
+  </si>
+  <si>
+    <t>Sheet #</t>
+  </si>
+  <si>
+    <t>Table of Contents</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>GDP</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>SimSummary_historical</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>SimSummary_historical_short</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>SimulationParms_forward</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>SimulationParms_historical</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>SimulationParms_historical_old</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Reference assumption</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
     <numFmt numFmtId="166" formatCode="0.000%"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0.000000000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -591,6 +688,14 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -715,11 +820,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -884,6 +990,71 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -902,6 +1073,27 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -911,12 +1103,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -950,65 +1145,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1512,6 +1654,463 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F8527B2-AD70-409F-A374-D231885E077B}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="84" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="84" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="85" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="86" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="85" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="86" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="85" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" s="86" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="85" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="86" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="85" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="86" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="85" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="86" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="85" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" s="86" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="85" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" s="86" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="85" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10" s="86" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" location="'GDP'!A1" display="GDP" xr:uid="{7B620BEF-03E6-463A-987A-DA86940000F6}"/>
+    <hyperlink ref="B3" location="'Stock'!A1" display="Stock" xr:uid="{7DCE4BE4-3DAD-4BF9-8EDC-FEA3CA0EC5D5}"/>
+    <hyperlink ref="B4" location="'SimSummary_historical'!A1" display="SimSummary_historical" xr:uid="{3737C865-CA72-4DE2-A132-0ACEA7D3C1AC}"/>
+    <hyperlink ref="B5" location="'SimSummary_historical_short'!A1" display="SimSummary_historical_short" xr:uid="{1C4DCB0A-CE17-481D-97CD-A5498828FD31}"/>
+    <hyperlink ref="B6" location="'SimulationParms_forward'!A1" display="SimulationParms_forward" xr:uid="{2C4319B6-BAA2-4C59-A6D2-8BC902636680}"/>
+    <hyperlink ref="B7" location="'SimulationParms_historical'!A1" display="SimulationParms_historical" xr:uid="{642A0CA1-CEF6-46B7-B055-A242647E3E55}"/>
+    <hyperlink ref="B8" location="'SimulationParms_historical_old'!A1" display="SimulationParms_historical_old" xr:uid="{1A062A69-ED2E-4344-AB9A-B5BF7F22AA6D}"/>
+    <hyperlink ref="B9" location="'Reference assumption'!A1" display="Reference assumption" xr:uid="{FF055582-AD6C-4C4C-9F6A-F144289A9AC0}"/>
+    <hyperlink ref="B10" location="'Sheet1'!A1" display="Sheet1" xr:uid="{2E3B7C82-9E59-4559-9BAA-293DB5685EC4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="B2:P8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>62</v>
+      </c>
+      <c r="F3">
+        <v>6.2965870509858093E-2</v>
+      </c>
+      <c r="G3">
+        <v>9.8820924995153395E-2</v>
+      </c>
+      <c r="H3">
+        <v>5.8064836770397601E-2</v>
+      </c>
+      <c r="I3">
+        <v>5.7186013768264099E-2</v>
+      </c>
+      <c r="J3">
+        <v>8.7197703707278598E-2</v>
+      </c>
+      <c r="K3">
+        <v>-0.13076106133601001</v>
+      </c>
+      <c r="L3">
+        <v>0.34148166563174398</v>
+      </c>
+      <c r="M3">
+        <v>0.47224272696775399</v>
+      </c>
+      <c r="N3">
+        <v>0.58119781062202902</v>
+      </c>
+      <c r="O3">
+        <v>0.221544658711429</v>
+      </c>
+      <c r="P3">
+        <v>1.2550270024660699E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1500</v>
+      </c>
+      <c r="F4">
+        <v>3.5552886122222301E-2</v>
+      </c>
+      <c r="G4">
+        <v>4.0148244712954403E-2</v>
+      </c>
+      <c r="H4">
+        <v>3.4194814497647101E-2</v>
+      </c>
+      <c r="I4">
+        <v>3.5246186175857501E-2</v>
+      </c>
+      <c r="J4">
+        <v>3.9717574412858503E-2</v>
+      </c>
+      <c r="K4">
+        <v>-0.123488094704773</v>
+      </c>
+      <c r="L4">
+        <v>0.16451603571780299</v>
+      </c>
+      <c r="M4">
+        <v>0.288004130422577</v>
+      </c>
+      <c r="N4">
+        <v>4.7369488451365502E-2</v>
+      </c>
+      <c r="O4">
+        <v>0.143257225626166</v>
+      </c>
+      <c r="P4">
+        <v>1.03662322101821E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>62</v>
+      </c>
+      <c r="F5">
+        <v>2.98063847473586E-2</v>
+      </c>
+      <c r="G5">
+        <v>2.5442282101289099E-2</v>
+      </c>
+      <c r="H5">
+        <v>3.04219805491023E-2</v>
+      </c>
+      <c r="I5">
+        <v>3.0665197609721501E-2</v>
+      </c>
+      <c r="J5">
+        <v>1.9737504970083902E-2</v>
+      </c>
+      <c r="K5">
+        <v>-4.1467161477593502E-2</v>
+      </c>
+      <c r="L5">
+        <v>8.8435952674173299E-2</v>
+      </c>
+      <c r="M5">
+        <v>0.129903114151766</v>
+      </c>
+      <c r="N5">
+        <v>-0.32058521689709202</v>
+      </c>
+      <c r="O5">
+        <v>0.27805982513156502</v>
+      </c>
+      <c r="P5">
+        <v>3.23117305803839E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1500</v>
+      </c>
+      <c r="F6">
+        <v>3.09034449294909E-2</v>
+      </c>
+      <c r="G6">
+        <v>2.1362621177804301E-2</v>
+      </c>
+      <c r="H6">
+        <v>3.3012378959294202E-2</v>
+      </c>
+      <c r="I6">
+        <v>3.2355747246079897E-2</v>
+      </c>
+      <c r="J6">
+        <v>1.8432211074052698E-2</v>
+      </c>
+      <c r="K6">
+        <v>-5.1403517682694098E-2</v>
+      </c>
+      <c r="L6">
+        <v>8.4344658680667497E-2</v>
+      </c>
+      <c r="M6">
+        <v>0.13574817636336101</v>
+      </c>
+      <c r="N6">
+        <v>-0.68642058074856505</v>
+      </c>
+      <c r="O6">
+        <v>0.76248592777908497</v>
+      </c>
+      <c r="P6" s="23">
+        <v>5.5158050701982703E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>62</v>
+      </c>
+      <c r="F7">
+        <v>0.103610955379368</v>
+      </c>
+      <c r="G7">
+        <v>0.15671132168063601</v>
+      </c>
+      <c r="H7">
+        <v>0.12681852649535</v>
+      </c>
+      <c r="I7">
+        <v>0.110780128453138</v>
+      </c>
+      <c r="J7">
+        <v>0.14967329512983399</v>
+      </c>
+      <c r="K7">
+        <v>-0.304004515060952</v>
+      </c>
+      <c r="L7">
+        <v>0.47735564947318498</v>
+      </c>
+      <c r="M7">
+        <v>0.78136016453413804</v>
+      </c>
+      <c r="N7">
+        <v>-0.38427129777646002</v>
+      </c>
+      <c r="O7">
+        <v>2.5557936764393201E-2</v>
+      </c>
+      <c r="P7">
+        <v>1.9902357755808401E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1500</v>
+      </c>
+      <c r="F8">
+        <v>0.107097152997913</v>
+      </c>
+      <c r="G8">
+        <v>0.16876749833910001</v>
+      </c>
+      <c r="H8">
+        <v>0.10694264976382201</v>
+      </c>
+      <c r="I8">
+        <v>0.10890629785990499</v>
+      </c>
+      <c r="J8">
+        <v>0.16081901091225301</v>
+      </c>
+      <c r="K8">
+        <v>-0.51257958073309695</v>
+      </c>
+      <c r="L8">
+        <v>0.76889643336060598</v>
+      </c>
+      <c r="M8">
+        <v>1.2814760140937</v>
+      </c>
+      <c r="N8">
+        <v>-0.120652222022161</v>
+      </c>
+      <c r="O8">
+        <v>0.49580980674382502</v>
+      </c>
+      <c r="P8">
+        <v>4.3575580696561603E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N13"/>
   <sheetViews>
@@ -1531,40 +2130,40 @@
   <sheetData>
     <row r="2" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65" t="s">
+      <c r="G3" s="90"/>
+      <c r="H3" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="65"/>
+      <c r="I3" s="90"/>
       <c r="J3" s="7"/>
       <c r="K3" s="1" t="s">
         <v>0</v>
@@ -1581,10 +2180,10 @@
     </row>
     <row r="4" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="90"/>
       <c r="F4" s="10" t="s">
         <v>8</v>
       </c>
@@ -1615,7 +2214,7 @@
         <v>17</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F5" s="9">
         <v>4.2999999999999997E-2</v>
@@ -1643,7 +2242,7 @@
         <v>19</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F6" s="9">
         <v>4.9000000000000002E-2</v>
@@ -1681,7 +2280,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F7" s="13">
         <v>4.8000000000000001E-2</v>
@@ -1783,7 +2382,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:O8"/>
   <sheetViews>
@@ -1803,40 +2402,40 @@
   <sheetData>
     <row r="2" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="87" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="67"/>
-      <c r="E3" s="66" t="s">
+      <c r="D3" s="92"/>
+      <c r="E3" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="67"/>
-      <c r="G3" s="65" t="s">
+      <c r="F3" s="92"/>
+      <c r="G3" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65" t="s">
+      <c r="H3" s="90"/>
+      <c r="I3" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="65"/>
+      <c r="J3" s="90"/>
       <c r="K3" s="7"/>
       <c r="L3" s="1" t="s">
         <v>0</v>
@@ -1853,7 +2452,7 @@
     </row>
     <row r="4" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="64"/>
+      <c r="B4" s="89"/>
       <c r="C4" s="10" t="s">
         <v>23</v>
       </c>
@@ -1985,12 +2584,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2003,42 +2602,42 @@
   <sheetData>
     <row r="2" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="71" t="s">
-        <v>134</v>
-      </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
+      <c r="B2" s="98" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
       <c r="J2" s="26"/>
       <c r="K2" s="26"/>
     </row>
     <row r="3" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
-      <c r="B3" s="95"/>
-      <c r="C3" s="97" t="s">
-        <v>138</v>
-      </c>
-      <c r="D3" s="84" t="s">
-        <v>145</v>
-      </c>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="97" t="s">
-        <v>139</v>
+      <c r="B3" s="93"/>
+      <c r="C3" s="95" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="96" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="95" t="s">
+        <v>137</v>
       </c>
       <c r="J3" s="57"/>
       <c r="K3" s="26"/>
     </row>
     <row r="4" spans="1:17" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26"/>
-      <c r="B4" s="96"/>
-      <c r="C4" s="64"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="89"/>
       <c r="D4" s="11" t="s">
         <v>127</v>
       </c>
@@ -2046,7 +2645,7 @@
         <v>128</v>
       </c>
       <c r="F4" s="56" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>129</v>
@@ -2054,75 +2653,75 @@
       <c r="H4" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="I4" s="98"/>
+      <c r="I4" s="99"/>
       <c r="J4" s="57"/>
       <c r="K4" s="26"/>
     </row>
     <row r="5" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26"/>
-      <c r="B5" s="68" t="s">
-        <v>135</v>
-      </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="100"/>
+      <c r="B5" s="100" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="71"/>
       <c r="K5" s="26"/>
     </row>
     <row r="6" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26"/>
-      <c r="B6" s="86" t="s">
-        <v>132</v>
+      <c r="B6" s="62" t="s">
+        <v>147</v>
       </c>
       <c r="C6" s="9">
+        <v>10</v>
+      </c>
+      <c r="D6" s="66">
+        <v>6</v>
+      </c>
+      <c r="E6" s="66">
         <v>9</v>
       </c>
-      <c r="D6" s="90">
-        <v>6</v>
-      </c>
-      <c r="E6" s="90">
-        <v>9</v>
-      </c>
-      <c r="F6" s="90">
+      <c r="F6" s="66">
         <v>10</v>
       </c>
-      <c r="G6" s="91">
+      <c r="G6" s="67">
         <v>12</v>
       </c>
-      <c r="H6" s="91">
+      <c r="H6" s="67">
         <v>15</v>
       </c>
       <c r="I6" s="9">
-        <v>0.38</v>
+        <v>0.52</v>
       </c>
       <c r="J6" s="21"/>
       <c r="K6" s="26"/>
     </row>
     <row r="7" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26"/>
-      <c r="B7" s="87" t="s">
-        <v>140</v>
+      <c r="B7" s="63" t="s">
+        <v>138</v>
       </c>
       <c r="C7" s="9">
         <v>3.7</v>
       </c>
-      <c r="D7" s="88">
+      <c r="D7" s="64">
         <v>1.92</v>
       </c>
-      <c r="E7" s="88">
+      <c r="E7" s="64">
         <v>2.54</v>
       </c>
-      <c r="F7" s="88">
+      <c r="F7" s="64">
         <v>3</v>
       </c>
-      <c r="G7" s="89">
+      <c r="G7" s="65">
         <v>3.58</v>
       </c>
-      <c r="H7" s="89">
+      <c r="H7" s="65">
         <v>4.6100000000000003</v>
       </c>
       <c r="I7" s="9">
@@ -2133,25 +2732,25 @@
     </row>
     <row r="8" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26"/>
-      <c r="B8" s="87" t="s">
-        <v>141</v>
+      <c r="B8" s="63" t="s">
+        <v>139</v>
       </c>
       <c r="C8" s="9">
         <v>20.2</v>
       </c>
-      <c r="D8" s="88">
+      <c r="D8" s="64">
         <v>12.69</v>
       </c>
-      <c r="E8" s="88">
+      <c r="E8" s="64">
         <v>16.079999999999998</v>
       </c>
-      <c r="F8" s="88">
+      <c r="F8" s="64">
         <v>19.36</v>
       </c>
-      <c r="G8" s="89">
+      <c r="G8" s="65">
         <v>23.78</v>
       </c>
-      <c r="H8" s="89">
+      <c r="H8" s="65">
         <v>33</v>
       </c>
       <c r="I8" s="9">
@@ -2162,17 +2761,17 @@
     </row>
     <row r="9" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26"/>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="100"/>
+      <c r="C9" s="101"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="102"/>
+      <c r="J9" s="71"/>
       <c r="K9" s="26"/>
     </row>
     <row r="10" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2208,7 +2807,7 @@
         <f>L10</f>
         <v>0.38319999999999999</v>
       </c>
-      <c r="J10" s="101"/>
+      <c r="J10" s="72"/>
       <c r="K10">
         <v>2.9806384747358597E-2</v>
       </c>
@@ -2234,7 +2833,7 @@
     <row r="11" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>
       <c r="B11" s="28" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="C11" s="16">
         <f t="shared" ref="C11:C13" si="1">K11</f>
@@ -2264,7 +2863,7 @@
         <f t="shared" ref="I11:I13" si="7">L11</f>
         <v>0.90739999999999998</v>
       </c>
-      <c r="J11" s="101"/>
+      <c r="J11" s="72"/>
       <c r="K11">
         <v>2.5442282101289147E-2</v>
       </c>
@@ -2320,7 +2919,7 @@
         <f t="shared" si="7"/>
         <v>0.87519999999999998</v>
       </c>
-      <c r="J12" s="101"/>
+      <c r="J12" s="72"/>
       <c r="K12">
         <v>-0.32850068057267229</v>
       </c>
@@ -2376,7 +2975,7 @@
         <f t="shared" si="7"/>
         <v>0.45979999999999999</v>
       </c>
-      <c r="J13" s="101"/>
+      <c r="J13" s="72"/>
       <c r="K13">
         <v>0.3864181585073152</v>
       </c>
@@ -2401,65 +3000,65 @@
     </row>
     <row r="14" spans="1:17" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
-      <c r="B14" s="92"/>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="93"/>
-      <c r="G14" s="93"/>
-      <c r="H14" s="93"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
       <c r="I14" s="26"/>
       <c r="J14" s="26"/>
     </row>
     <row r="15" spans="1:17" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
-      <c r="B15" s="92"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="93"/>
-      <c r="E15" s="93"/>
-      <c r="F15" s="93"/>
-      <c r="G15" s="93"/>
-      <c r="H15" s="93"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
       <c r="I15" s="26"/>
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26"/>
-      <c r="B16" s="71" t="s">
-        <v>136</v>
-      </c>
-      <c r="C16" s="71"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71"/>
-      <c r="H16" s="71"/>
-      <c r="I16" s="71"/>
+      <c r="B16" s="98" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" s="98"/>
+      <c r="D16" s="98"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="98"/>
+      <c r="H16" s="98"/>
+      <c r="I16" s="98"/>
       <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="26"/>
-      <c r="B17" s="95"/>
-      <c r="C17" s="97" t="s">
-        <v>138</v>
-      </c>
-      <c r="D17" s="84" t="s">
-        <v>145</v>
-      </c>
-      <c r="E17" s="94"/>
-      <c r="F17" s="94"/>
-      <c r="G17" s="94"/>
-      <c r="H17" s="94"/>
-      <c r="I17" s="97" t="s">
-        <v>139</v>
+      <c r="B17" s="93"/>
+      <c r="C17" s="95" t="s">
+        <v>136</v>
+      </c>
+      <c r="D17" s="96" t="s">
+        <v>143</v>
+      </c>
+      <c r="E17" s="97"/>
+      <c r="F17" s="97"/>
+      <c r="G17" s="97"/>
+      <c r="H17" s="97"/>
+      <c r="I17" s="95" t="s">
+        <v>137</v>
       </c>
       <c r="J17" s="57"/>
       <c r="K17" s="26"/>
     </row>
     <row r="18" spans="1:17" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
-      <c r="B18" s="96"/>
-      <c r="C18" s="64"/>
+      <c r="B18" s="94"/>
+      <c r="C18" s="89"/>
       <c r="D18" s="11" t="s">
         <v>127</v>
       </c>
@@ -2467,7 +3066,7 @@
         <v>128</v>
       </c>
       <c r="F18" s="56" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>129</v>
@@ -2475,7 +3074,7 @@
       <c r="H18" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="I18" s="98"/>
+      <c r="I18" s="99"/>
       <c r="J18" s="57"/>
       <c r="K18" s="26"/>
     </row>
@@ -2512,7 +3111,7 @@
         <f>L19</f>
         <v>0.40379999999999999</v>
       </c>
-      <c r="J19" s="101"/>
+      <c r="J19" s="72"/>
       <c r="K19">
         <v>0.10361095537936856</v>
       </c>
@@ -2538,7 +3137,7 @@
     <row r="20" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
       <c r="B20" s="28" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="C20" s="16">
         <f t="shared" ref="C20:C22" si="12">K20</f>
@@ -2568,7 +3167,7 @@
         <f t="shared" ref="I20:I22" si="14">L20</f>
         <v>0.18559999999999999</v>
       </c>
-      <c r="J20" s="101"/>
+      <c r="J20" s="72"/>
       <c r="K20">
         <v>0.15671132168063609</v>
       </c>
@@ -2624,7 +3223,7 @@
         <f t="shared" si="14"/>
         <v>0.1138</v>
       </c>
-      <c r="J21" s="101"/>
+      <c r="J21" s="72"/>
       <c r="K21">
         <v>-0.39375921343445103</v>
       </c>
@@ -2680,7 +3279,7 @@
         <f t="shared" si="14"/>
         <v>0.51700000000000002</v>
       </c>
-      <c r="J22" s="101"/>
+      <c r="J22" s="72"/>
       <c r="K22">
         <v>0.12556966109173073</v>
       </c>
@@ -2705,65 +3304,65 @@
     </row>
     <row r="23" spans="1:17" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
-      <c r="B23" s="92"/>
-      <c r="C23" s="93"/>
-      <c r="D23" s="93"/>
-      <c r="E23" s="93"/>
-      <c r="F23" s="93"/>
-      <c r="G23" s="93"/>
-      <c r="H23" s="93"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="69"/>
       <c r="I23" s="26"/>
       <c r="J23" s="26"/>
     </row>
     <row r="24" spans="1:17" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
-      <c r="B24" s="92"/>
-      <c r="C24" s="93"/>
-      <c r="D24" s="93"/>
-      <c r="E24" s="93"/>
-      <c r="F24" s="93"/>
-      <c r="G24" s="93"/>
-      <c r="H24" s="93"/>
+      <c r="B24" s="68"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
       <c r="I24" s="26"/>
       <c r="J24" s="26"/>
     </row>
     <row r="25" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26"/>
-      <c r="B25" s="71" t="s">
-        <v>137</v>
-      </c>
-      <c r="C25" s="72"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
-      <c r="H25" s="72"/>
+      <c r="B25" s="98" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="103"/>
+      <c r="D25" s="103"/>
+      <c r="E25" s="103"/>
+      <c r="F25" s="103"/>
+      <c r="G25" s="103"/>
+      <c r="H25" s="103"/>
       <c r="I25" s="26"/>
       <c r="J25" s="26"/>
     </row>
     <row r="26" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
-      <c r="B26" s="95"/>
-      <c r="C26" s="97" t="s">
-        <v>138</v>
-      </c>
-      <c r="D26" s="84" t="s">
-        <v>145</v>
-      </c>
-      <c r="E26" s="94"/>
-      <c r="F26" s="94"/>
-      <c r="G26" s="94"/>
-      <c r="H26" s="94"/>
-      <c r="I26" s="97" t="s">
-        <v>139</v>
+      <c r="B26" s="93"/>
+      <c r="C26" s="95" t="s">
+        <v>136</v>
+      </c>
+      <c r="D26" s="96" t="s">
+        <v>143</v>
+      </c>
+      <c r="E26" s="97"/>
+      <c r="F26" s="97"/>
+      <c r="G26" s="97"/>
+      <c r="H26" s="97"/>
+      <c r="I26" s="95" t="s">
+        <v>137</v>
       </c>
       <c r="J26" s="57"/>
       <c r="K26" s="26"/>
     </row>
     <row r="27" spans="1:17" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
-      <c r="B27" s="96"/>
-      <c r="C27" s="64"/>
+      <c r="B27" s="94"/>
+      <c r="C27" s="89"/>
       <c r="D27" s="11" t="s">
         <v>127</v>
       </c>
@@ -2771,7 +3370,7 @@
         <v>128</v>
       </c>
       <c r="F27" s="56" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G27" s="11" t="s">
         <v>129</v>
@@ -2779,7 +3378,7 @@
       <c r="H27" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="I27" s="98"/>
+      <c r="I27" s="99"/>
       <c r="J27" s="57"/>
       <c r="K27" s="26"/>
     </row>
@@ -2812,11 +3411,11 @@
         <f t="shared" ref="H28:H31" si="18">Q28</f>
         <v>8.7562901660437939E-2</v>
       </c>
-      <c r="I28" s="99">
+      <c r="I28" s="70">
         <f>L28</f>
         <v>0.49330000000000002</v>
       </c>
-      <c r="J28" s="102"/>
+      <c r="J28" s="73"/>
       <c r="K28">
         <v>6.5553415906824078E-2</v>
       </c>
@@ -2842,7 +3441,7 @@
     <row r="29" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
       <c r="B29" s="28" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="C29" s="16">
         <f t="shared" ref="C29:C31" si="19">K29</f>
@@ -2868,11 +3467,11 @@
         <f t="shared" si="18"/>
         <v>0.12356274041515744</v>
       </c>
-      <c r="I29" s="99">
+      <c r="I29" s="70">
         <f t="shared" ref="I29:I31" si="21">L29</f>
         <v>0.14199999999999999</v>
       </c>
-      <c r="J29" s="102"/>
+      <c r="J29" s="73"/>
       <c r="K29">
         <v>9.6320844630497005E-2</v>
       </c>
@@ -2924,11 +3523,11 @@
         <f t="shared" si="18"/>
         <v>0.69699592458608917</v>
       </c>
-      <c r="I30" s="99">
+      <c r="I30" s="70">
         <f t="shared" si="21"/>
         <v>0.9093</v>
       </c>
-      <c r="J30" s="102"/>
+      <c r="J30" s="73"/>
       <c r="K30">
         <v>0.59511685935455705</v>
       </c>
@@ -2980,11 +3579,11 @@
         <f t="shared" si="18"/>
         <v>1.0976953780626306</v>
       </c>
-      <c r="I31" s="99">
+      <c r="I31" s="70">
         <f t="shared" si="21"/>
         <v>0.88219999999999998</v>
       </c>
-      <c r="J31" s="102"/>
+      <c r="J31" s="73"/>
       <c r="K31">
         <v>0.63193703796576051</v>
       </c>
@@ -3056,8 +3655,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B16:I16"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="D26:H26"/>
@@ -3073,17 +3670,643 @@
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:H17"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B16:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196F361E-FFA9-4D39-A4D7-75BA43ABD3BB}">
+  <dimension ref="A2:O28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="80" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
+      <c r="B2" s="98" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+    </row>
+    <row r="3" spans="1:15" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="74" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="74" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" s="75"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="26"/>
+    </row>
+    <row r="4" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26"/>
+      <c r="B4" s="105" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="105"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="26"/>
+    </row>
+    <row r="5" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26"/>
+      <c r="B5" s="62" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="9">
+        <v>10</v>
+      </c>
+      <c r="D5" s="66">
+        <v>10</v>
+      </c>
+      <c r="E5" s="9" t="str">
+        <f>F5&amp;"th"</f>
+        <v>52th</v>
+      </c>
+      <c r="F5" s="82">
+        <f>ROUND(G5*100, 0)</f>
+        <v>52</v>
+      </c>
+      <c r="G5" s="72">
+        <v>0.52</v>
+      </c>
+      <c r="H5" s="21"/>
+      <c r="I5" s="26"/>
+    </row>
+    <row r="6" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26"/>
+      <c r="B6" s="62" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="9">
+        <v>10</v>
+      </c>
+      <c r="D6" s="66">
+        <v>11</v>
+      </c>
+      <c r="E6" s="9" t="str">
+        <f t="shared" ref="E6:E8" si="0">F6&amp;"th"</f>
+        <v>40th</v>
+      </c>
+      <c r="F6" s="82">
+        <f t="shared" ref="F6:F19" si="1">ROUND(G6*100, 0)</f>
+        <v>40</v>
+      </c>
+      <c r="G6" s="72">
+        <v>0.4</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="26"/>
+    </row>
+    <row r="7" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="26"/>
+      <c r="B7" s="63" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" s="9">
+        <v>3.7</v>
+      </c>
+      <c r="D7" s="64">
+        <v>3</v>
+      </c>
+      <c r="E7" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>79th</v>
+      </c>
+      <c r="F7" s="82">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="G7" s="72">
+        <v>0.79</v>
+      </c>
+      <c r="H7" s="21"/>
+      <c r="I7" s="26"/>
+    </row>
+    <row r="8" spans="1:15" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="26"/>
+      <c r="B8" s="63" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="9">
+        <v>20.2</v>
+      </c>
+      <c r="D8" s="64">
+        <v>19.36</v>
+      </c>
+      <c r="E8" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>57th</v>
+      </c>
+      <c r="F8" s="82">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="G8" s="72">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H8" s="21"/>
+      <c r="I8" s="26"/>
+    </row>
+    <row r="9" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="26"/>
+      <c r="B9" s="105" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="105"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="82"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="26"/>
+    </row>
+    <row r="10" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="26"/>
+      <c r="B10" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="16">
+        <f>I10</f>
+        <v>2.9806384747358597E-2</v>
+      </c>
+      <c r="D10" s="16">
+        <f>M10</f>
+        <v>3.0747711721745577E-2</v>
+      </c>
+      <c r="E10" s="83" t="str">
+        <f>F10&amp;"th"</f>
+        <v>38th</v>
+      </c>
+      <c r="F10" s="82">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="G10" s="72">
+        <v>0.38319999999999999</v>
+      </c>
+      <c r="H10" s="21"/>
+      <c r="I10">
+        <v>2.9806384747358597E-2</v>
+      </c>
+      <c r="J10">
+        <v>0.38319999999999999</v>
+      </c>
+      <c r="K10">
+        <v>2.4768728085590375E-2</v>
+      </c>
+      <c r="L10">
+        <v>2.8533286192731301E-2</v>
+      </c>
+      <c r="M10">
+        <v>3.0747711721745577E-2</v>
+      </c>
+      <c r="N10">
+        <v>3.2881286556135966E-2</v>
+      </c>
+      <c r="O10">
+        <v>3.5926090354154672E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="26"/>
+      <c r="B11" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" s="16">
+        <f>I11</f>
+        <v>2.5442282101289147E-2</v>
+      </c>
+      <c r="D11" s="16">
+        <f>M11</f>
+        <v>2.1785273183534459E-2</v>
+      </c>
+      <c r="E11" s="83" t="str">
+        <f>F11&amp;"th"</f>
+        <v>91th</v>
+      </c>
+      <c r="F11" s="82">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="G11" s="72">
+        <v>0.90739999999999998</v>
+      </c>
+      <c r="I11">
+        <v>2.5442282101289147E-2</v>
+      </c>
+      <c r="J11">
+        <v>0.90739999999999998</v>
+      </c>
+      <c r="K11">
+        <v>1.7417916879809002E-2</v>
+      </c>
+      <c r="L11">
+        <v>1.9915948778730215E-2</v>
+      </c>
+      <c r="M11">
+        <v>2.1785273183534459E-2</v>
+      </c>
+      <c r="N11">
+        <v>2.3631726332846083E-2</v>
+      </c>
+      <c r="O11">
+        <v>2.6258952600929919E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="26"/>
+      <c r="B12" s="104" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="104"/>
+      <c r="D12" s="104"/>
+      <c r="E12" s="104"/>
+      <c r="F12" s="82"/>
+    </row>
+    <row r="13" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="26"/>
+      <c r="B13" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="16">
+        <f>I13</f>
+        <v>0.10361095537936856</v>
+      </c>
+      <c r="D13" s="16">
+        <f>M13</f>
+        <v>0.10915892800675997</v>
+      </c>
+      <c r="E13" s="27" t="str">
+        <f>F13&amp;"th"</f>
+        <v>40th</v>
+      </c>
+      <c r="F13" s="82">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="G13" s="72">
+        <v>0.40379999999999999</v>
+      </c>
+      <c r="H13" s="21"/>
+      <c r="I13">
+        <v>0.10361095537936856</v>
+      </c>
+      <c r="J13">
+        <v>0.40379999999999999</v>
+      </c>
+      <c r="K13">
+        <v>7.1391375958434186E-2</v>
+      </c>
+      <c r="L13">
+        <v>9.4060909335626122E-2</v>
+      </c>
+      <c r="M13">
+        <v>0.10915892800675997</v>
+      </c>
+      <c r="N13">
+        <v>0.12491717739787672</v>
+      </c>
+      <c r="O13">
+        <v>0.14602850638300593</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="26"/>
+      <c r="B14" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="16">
+        <f>I14</f>
+        <v>0.15671132168063609</v>
+      </c>
+      <c r="D14" s="16">
+        <f>M14</f>
+        <v>0.17219167396714474</v>
+      </c>
+      <c r="E14" s="27" t="str">
+        <f t="shared" ref="E14:E15" si="2">F14&amp;"th"</f>
+        <v>19th</v>
+      </c>
+      <c r="F14" s="82">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="G14" s="72">
+        <v>0.18559999999999999</v>
+      </c>
+      <c r="H14" s="21"/>
+      <c r="I14">
+        <v>0.15671132168063609</v>
+      </c>
+      <c r="J14">
+        <v>0.18559999999999999</v>
+      </c>
+      <c r="K14">
+        <v>0.14406074705632738</v>
+      </c>
+      <c r="L14">
+        <v>0.16022082355905881</v>
+      </c>
+      <c r="M14">
+        <v>0.17219167396714474</v>
+      </c>
+      <c r="N14">
+        <v>0.18462651990350848</v>
+      </c>
+      <c r="O14">
+        <v>0.20399436980682509</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="26"/>
+      <c r="B15" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="C15" s="17">
+        <f>I15</f>
+        <v>0.12556966109173073</v>
+      </c>
+      <c r="D15" s="17">
+        <f>M15</f>
+        <v>9.5360022085102081E-2</v>
+      </c>
+      <c r="E15" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v>52th</v>
+      </c>
+      <c r="F15" s="82">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="G15" s="72">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="H15" s="21"/>
+      <c r="I15">
+        <v>0.12556966109173073</v>
+      </c>
+      <c r="J15">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="K15">
+        <v>-0.65353566352602388</v>
+      </c>
+      <c r="L15">
+        <v>-0.27599607268647997</v>
+      </c>
+      <c r="M15">
+        <v>9.5360022085102081E-2</v>
+      </c>
+      <c r="N15">
+        <v>0.61047043379809773</v>
+      </c>
+      <c r="O15">
+        <v>1.6099757864094923</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26"/>
+      <c r="B16" s="104" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="104"/>
+      <c r="D16" s="104"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="82"/>
+    </row>
+    <row r="17" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="26"/>
+      <c r="B17" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="16">
+        <f>I17</f>
+        <v>6.5553415906824078E-2</v>
+      </c>
+      <c r="D17" s="16">
+        <f>M17</f>
+        <v>6.5808776482831122E-2</v>
+      </c>
+      <c r="E17" s="27" t="str">
+        <f>F17&amp;"th"</f>
+        <v>49th</v>
+      </c>
+      <c r="F17" s="82">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="G17" s="72">
+        <v>0.49330000000000002</v>
+      </c>
+      <c r="H17" s="21"/>
+      <c r="I17">
+        <v>6.5553415906824078E-2</v>
+      </c>
+      <c r="J17">
+        <v>0.49330000000000002</v>
+      </c>
+      <c r="K17">
+        <v>4.3624943823150991E-2</v>
+      </c>
+      <c r="L17">
+        <v>5.6991371575956309E-2</v>
+      </c>
+      <c r="M17">
+        <v>6.5808776482831122E-2</v>
+      </c>
+      <c r="N17">
+        <v>7.4921163632362925E-2</v>
+      </c>
+      <c r="O17">
+        <v>8.7562901660437939E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="26"/>
+      <c r="B18" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" s="16">
+        <f>I18</f>
+        <v>9.6320844630497005E-2</v>
+      </c>
+      <c r="D18" s="16">
+        <f>M18</f>
+        <v>0.1064011381672044</v>
+      </c>
+      <c r="E18" s="27" t="str">
+        <f t="shared" ref="E18:E19" si="3">F18&amp;"th"</f>
+        <v>14th</v>
+      </c>
+      <c r="F18" s="82">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="G18" s="72">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="H18" s="21"/>
+      <c r="I18">
+        <v>9.6320844630497005E-2</v>
+      </c>
+      <c r="J18">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="K18">
+        <v>9.1101250947868376E-2</v>
+      </c>
+      <c r="L18">
+        <v>9.9869017757115666E-2</v>
+      </c>
+      <c r="M18">
+        <v>0.1064011381672044</v>
+      </c>
+      <c r="N18">
+        <v>0.11354558088574518</v>
+      </c>
+      <c r="O18">
+        <v>0.12356274041515744</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="26"/>
+      <c r="B19" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="C19" s="17">
+        <f>I19</f>
+        <v>0.63193703796576051</v>
+      </c>
+      <c r="D19" s="17">
+        <f>M19</f>
+        <v>-0.15602928488355383</v>
+      </c>
+      <c r="E19" s="27" t="str">
+        <f t="shared" si="3"/>
+        <v>88th</v>
+      </c>
+      <c r="F19" s="82">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="G19" s="72">
+        <v>0.88219999999999998</v>
+      </c>
+      <c r="H19" s="21"/>
+      <c r="I19">
+        <v>0.63193703796576051</v>
+      </c>
+      <c r="J19">
+        <v>0.88219999999999998</v>
+      </c>
+      <c r="K19">
+        <v>-0.77465178889245245</v>
+      </c>
+      <c r="L19">
+        <v>-0.46254905094589238</v>
+      </c>
+      <c r="M19">
+        <v>-0.15602928488355383</v>
+      </c>
+      <c r="N19">
+        <v>0.21759826456773934</v>
+      </c>
+      <c r="O19">
+        <v>1.0976953780626306</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="82"/>
+      <c r="G20" s="77"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+    </row>
+    <row r="21" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="77"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="81"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="81"/>
+      <c r="H28" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3115,32 +4338,32 @@
     <row r="2" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="26"/>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
       <c r="J2" s="26"/>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="26"/>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="106" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="73"/>
+      <c r="D3" s="106"/>
       <c r="E3" s="47"/>
-      <c r="F3" s="75" t="s">
+      <c r="F3" s="108" t="s">
         <v>126</v>
       </c>
-      <c r="G3" s="75"/>
+      <c r="G3" s="108"/>
       <c r="H3" s="37"/>
-      <c r="I3" s="76" t="s">
+      <c r="I3" s="109" t="s">
         <v>109</v>
       </c>
       <c r="J3" s="26"/>
@@ -3149,8 +4372,8 @@
     <row r="4" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="26"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="107"/>
       <c r="E4" s="41"/>
       <c r="F4" s="44" t="s">
         <v>99</v>
@@ -3159,14 +4382,14 @@
         <v>100</v>
       </c>
       <c r="H4" s="25"/>
-      <c r="I4" s="74"/>
+      <c r="I4" s="107"/>
       <c r="J4" s="26"/>
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="26"/>
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="106" t="s">
         <v>120</v>
       </c>
       <c r="D5" s="40" t="s">
@@ -3180,7 +4403,7 @@
         <v>102</v>
       </c>
       <c r="H5" s="43"/>
-      <c r="I5" s="82" t="s">
+      <c r="I5" s="115" t="s">
         <v>125</v>
       </c>
       <c r="J5" s="26"/>
@@ -3189,7 +4412,7 @@
     <row r="6" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="26"/>
-      <c r="C6" s="77"/>
+      <c r="C6" s="110"/>
       <c r="D6" s="40" t="s">
         <v>103</v>
       </c>
@@ -3201,14 +4424,14 @@
         <v>112</v>
       </c>
       <c r="H6" s="38"/>
-      <c r="I6" s="82"/>
+      <c r="I6" s="115"/>
       <c r="J6" s="26"/>
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="26"/>
-      <c r="C7" s="62"/>
+      <c r="C7" s="87"/>
       <c r="D7" s="45" t="s">
         <v>104</v>
       </c>
@@ -3220,14 +4443,14 @@
         <v>113</v>
       </c>
       <c r="H7" s="38"/>
-      <c r="I7" s="82"/>
+      <c r="I7" s="115"/>
       <c r="J7" s="26"/>
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="26"/>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="106" t="s">
         <v>121</v>
       </c>
       <c r="D8" s="40" t="s">
@@ -3241,7 +4464,7 @@
         <v>115</v>
       </c>
       <c r="H8" s="38"/>
-      <c r="I8" s="82" t="s">
+      <c r="I8" s="115" t="s">
         <v>123</v>
       </c>
       <c r="J8" s="26"/>
@@ -3250,7 +4473,7 @@
     <row r="9" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="26"/>
-      <c r="C9" s="62"/>
+      <c r="C9" s="87"/>
       <c r="D9" s="45" t="s">
         <v>106</v>
       </c>
@@ -3262,14 +4485,14 @@
         <v>117</v>
       </c>
       <c r="H9" s="39"/>
-      <c r="I9" s="82"/>
+      <c r="I9" s="115"/>
       <c r="J9" s="26"/>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="26"/>
-      <c r="C10" s="73" t="s">
+      <c r="C10" s="106" t="s">
         <v>122</v>
       </c>
       <c r="D10" s="19" t="s">
@@ -3283,7 +4506,7 @@
         <v>118</v>
       </c>
       <c r="H10" s="39"/>
-      <c r="I10" s="79" t="s">
+      <c r="I10" s="112" t="s">
         <v>124</v>
       </c>
       <c r="J10" s="26"/>
@@ -3292,7 +4515,7 @@
     <row r="11" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="26"/>
-      <c r="C11" s="77"/>
+      <c r="C11" s="110"/>
       <c r="D11" s="19" t="s">
         <v>106</v>
       </c>
@@ -3304,14 +4527,14 @@
         <v>119</v>
       </c>
       <c r="H11" s="39"/>
-      <c r="I11" s="80"/>
+      <c r="I11" s="113"/>
       <c r="J11" s="26"/>
       <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="26"/>
-      <c r="C12" s="62"/>
+      <c r="C12" s="87"/>
       <c r="D12" s="48" t="s">
         <v>108</v>
       </c>
@@ -3321,22 +4544,22 @@
       </c>
       <c r="G12" s="54"/>
       <c r="H12" s="46"/>
-      <c r="I12" s="81"/>
+      <c r="I12" s="114"/>
       <c r="J12" s="26"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="26"/>
-      <c r="C13" s="78" t="s">
-        <v>110</v>
-      </c>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="78"/>
+      <c r="C13" s="111" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" s="111"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="111"/>
       <c r="J13" s="26"/>
       <c r="K13" s="5"/>
     </row>
@@ -3398,7 +4621,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25CDD40-5261-46CC-961A-D80A3A8822ED}">
   <dimension ref="A1:K16"/>
   <sheetViews>
@@ -3435,32 +4658,32 @@
     <row r="2" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="26"/>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
       <c r="J2" s="26"/>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="26"/>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="106" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="73"/>
+      <c r="D3" s="106"/>
       <c r="E3" s="47"/>
-      <c r="F3" s="75" t="s">
+      <c r="F3" s="108" t="s">
         <v>126</v>
       </c>
-      <c r="G3" s="75"/>
+      <c r="G3" s="108"/>
       <c r="H3" s="37"/>
-      <c r="I3" s="76" t="s">
+      <c r="I3" s="109" t="s">
         <v>109</v>
       </c>
       <c r="J3" s="26"/>
@@ -3469,8 +4692,8 @@
     <row r="4" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="26"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="107"/>
       <c r="E4" s="57"/>
       <c r="F4" s="61" t="s">
         <v>99</v>
@@ -3479,14 +4702,14 @@
         <v>100</v>
       </c>
       <c r="H4" s="58"/>
-      <c r="I4" s="74"/>
+      <c r="I4" s="107"/>
       <c r="J4" s="26"/>
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="26"/>
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="106" t="s">
         <v>120</v>
       </c>
       <c r="D5" s="59" t="s">
@@ -3500,7 +4723,7 @@
         <v>102</v>
       </c>
       <c r="H5" s="43"/>
-      <c r="I5" s="82" t="s">
+      <c r="I5" s="115" t="s">
         <v>125</v>
       </c>
       <c r="J5" s="26"/>
@@ -3509,7 +4732,7 @@
     <row r="6" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="26"/>
-      <c r="C6" s="77"/>
+      <c r="C6" s="110"/>
       <c r="D6" s="59" t="s">
         <v>103</v>
       </c>
@@ -3521,14 +4744,14 @@
         <v>112</v>
       </c>
       <c r="H6" s="38"/>
-      <c r="I6" s="82"/>
+      <c r="I6" s="115"/>
       <c r="J6" s="26"/>
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="26"/>
-      <c r="C7" s="62"/>
+      <c r="C7" s="87"/>
       <c r="D7" s="60" t="s">
         <v>104</v>
       </c>
@@ -3540,14 +4763,14 @@
         <v>113</v>
       </c>
       <c r="H7" s="38"/>
-      <c r="I7" s="82"/>
+      <c r="I7" s="115"/>
       <c r="J7" s="26"/>
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="26"/>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="106" t="s">
         <v>121</v>
       </c>
       <c r="D8" s="59" t="s">
@@ -3561,7 +4784,7 @@
         <v>115</v>
       </c>
       <c r="H8" s="38"/>
-      <c r="I8" s="82" t="s">
+      <c r="I8" s="115" t="s">
         <v>123</v>
       </c>
       <c r="J8" s="26"/>
@@ -3570,7 +4793,7 @@
     <row r="9" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="26"/>
-      <c r="C9" s="62"/>
+      <c r="C9" s="87"/>
       <c r="D9" s="60" t="s">
         <v>106</v>
       </c>
@@ -3582,14 +4805,14 @@
         <v>117</v>
       </c>
       <c r="H9" s="39"/>
-      <c r="I9" s="82"/>
+      <c r="I9" s="115"/>
       <c r="J9" s="26"/>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="26"/>
-      <c r="C10" s="73" t="s">
+      <c r="C10" s="106" t="s">
         <v>122</v>
       </c>
       <c r="D10" s="19" t="s">
@@ -3603,7 +4826,7 @@
         <v>118</v>
       </c>
       <c r="H10" s="39"/>
-      <c r="I10" s="79" t="s">
+      <c r="I10" s="112" t="s">
         <v>124</v>
       </c>
       <c r="J10" s="26"/>
@@ -3612,7 +4835,7 @@
     <row r="11" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="26"/>
-      <c r="C11" s="77"/>
+      <c r="C11" s="110"/>
       <c r="D11" s="19" t="s">
         <v>106</v>
       </c>
@@ -3624,14 +4847,14 @@
         <v>119</v>
       </c>
       <c r="H11" s="39"/>
-      <c r="I11" s="80"/>
+      <c r="I11" s="113"/>
       <c r="J11" s="26"/>
       <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="26"/>
-      <c r="C12" s="62"/>
+      <c r="C12" s="87"/>
       <c r="D12" s="48" t="s">
         <v>108</v>
       </c>
@@ -3641,22 +4864,22 @@
       </c>
       <c r="G12" s="54"/>
       <c r="H12" s="46"/>
-      <c r="I12" s="81"/>
+      <c r="I12" s="114"/>
       <c r="J12" s="26"/>
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="26"/>
-      <c r="C13" s="78" t="s">
+      <c r="C13" s="111" t="s">
         <v>110</v>
       </c>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="78"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="111"/>
       <c r="J13" s="26"/>
       <c r="K13" s="5"/>
     </row>
@@ -3718,7 +4941,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
@@ -3751,17 +4974,17 @@
     </row>
     <row r="2" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
@@ -3797,7 +5020,7 @@
       <c r="C4" s="15">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="116" t="s">
         <v>48</v>
       </c>
       <c r="E4" s="5"/>
@@ -3807,7 +5030,7 @@
       <c r="G4" s="15">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="H4" s="83" t="s">
+      <c r="H4" s="116" t="s">
         <v>48</v>
       </c>
       <c r="I4" s="5"/>
@@ -3821,7 +5044,7 @@
       <c r="C5" s="15">
         <v>0.32</v>
       </c>
-      <c r="D5" s="83"/>
+      <c r="D5" s="116"/>
       <c r="E5" s="5"/>
       <c r="F5" s="14" t="s">
         <v>37</v>
@@ -3829,7 +5052,7 @@
       <c r="G5" s="36">
         <v>0.32</v>
       </c>
-      <c r="H5" s="83"/>
+      <c r="H5" s="116"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
@@ -3841,7 +5064,7 @@
       <c r="C6" s="15">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="D6" s="83"/>
+      <c r="D6" s="116"/>
       <c r="E6" s="5"/>
       <c r="F6" s="14" t="s">
         <v>39</v>
@@ -3849,7 +5072,7 @@
       <c r="G6" s="15">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="H6" s="83"/>
+      <c r="H6" s="116"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
@@ -3861,7 +5084,7 @@
       <c r="C7" s="15">
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="D7" s="83"/>
+      <c r="D7" s="116"/>
       <c r="E7" s="5"/>
       <c r="F7" s="14" t="s">
         <v>38</v>
@@ -3869,7 +5092,7 @@
       <c r="G7" s="15">
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="H7" s="83"/>
+      <c r="H7" s="116"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
@@ -3881,7 +5104,7 @@
       <c r="C8" s="15">
         <v>7.4000000000000003E-3</v>
       </c>
-      <c r="D8" s="83"/>
+      <c r="D8" s="116"/>
       <c r="E8" s="5"/>
       <c r="F8" s="14" t="s">
         <v>40</v>
@@ -3889,7 +5112,7 @@
       <c r="G8" s="15">
         <v>7.4000000000000003E-3</v>
       </c>
-      <c r="H8" s="83"/>
+      <c r="H8" s="116"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
@@ -3913,7 +5136,7 @@
       <c r="C10" s="15">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="D10" s="83" t="s">
+      <c r="D10" s="116" t="s">
         <v>50</v>
       </c>
       <c r="E10" s="5"/>
@@ -3923,7 +5146,7 @@
       <c r="G10" s="15">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="H10" s="83" t="s">
+      <c r="H10" s="116" t="s">
         <v>50</v>
       </c>
       <c r="I10" s="5"/>
@@ -3937,7 +5160,7 @@
       <c r="C11" s="15">
         <v>-1.4E-2</v>
       </c>
-      <c r="D11" s="83"/>
+      <c r="D11" s="116"/>
       <c r="E11" s="5"/>
       <c r="F11" s="14" t="s">
         <v>42</v>
@@ -3945,7 +5168,7 @@
       <c r="G11" s="15">
         <v>-1.4E-2</v>
       </c>
-      <c r="H11" s="83"/>
+      <c r="H11" s="116"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
@@ -3957,7 +5180,7 @@
       <c r="C12" s="15">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="D12" s="83"/>
+      <c r="D12" s="116"/>
       <c r="E12" s="5"/>
       <c r="F12" s="14" t="s">
         <v>43</v>
@@ -3965,7 +5188,7 @@
       <c r="G12" s="15">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="H12" s="83"/>
+      <c r="H12" s="116"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
@@ -3977,7 +5200,7 @@
       <c r="C13" s="16">
         <v>0.11899999999999999</v>
       </c>
-      <c r="D13" s="83"/>
+      <c r="D13" s="116"/>
       <c r="E13" s="5"/>
       <c r="F13" s="14" t="s">
         <v>44</v>
@@ -3985,7 +5208,7 @@
       <c r="G13" s="16">
         <v>0.11899999999999999</v>
       </c>
-      <c r="H13" s="83"/>
+      <c r="H13" s="116"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
@@ -4009,7 +5232,7 @@
       <c r="C15" s="16">
         <v>1.5699999999999999E-2</v>
       </c>
-      <c r="D15" s="83" t="s">
+      <c r="D15" s="116" t="s">
         <v>51</v>
       </c>
       <c r="E15" s="5"/>
@@ -4019,7 +5242,7 @@
       <c r="G15" s="16">
         <v>1.5699999999999999E-2</v>
       </c>
-      <c r="H15" s="85" t="s">
+      <c r="H15" s="117" t="s">
         <v>51</v>
       </c>
       <c r="I15" s="5"/>
@@ -4033,7 +5256,7 @@
       <c r="C16" s="16">
         <v>5.1400000000000001E-2</v>
       </c>
-      <c r="D16" s="83"/>
+      <c r="D16" s="116"/>
       <c r="E16" s="5"/>
       <c r="F16" s="14" t="s">
         <v>46</v>
@@ -4041,7 +5264,7 @@
       <c r="G16" s="16">
         <v>5.1400000000000001E-2</v>
       </c>
-      <c r="H16" s="85"/>
+      <c r="H16" s="117"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
@@ -4132,7 +5355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:M34"/>
   <sheetViews>
@@ -4278,348 +5501,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="B2:P8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K2" t="s">
-        <v>64</v>
-      </c>
-      <c r="L2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M2" t="s">
-        <v>66</v>
-      </c>
-      <c r="N2" t="s">
-        <v>67</v>
-      </c>
-      <c r="O2" t="s">
-        <v>68</v>
-      </c>
-      <c r="P2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>62</v>
-      </c>
-      <c r="F3">
-        <v>6.2965870509858093E-2</v>
-      </c>
-      <c r="G3">
-        <v>9.8820924995153395E-2</v>
-      </c>
-      <c r="H3">
-        <v>5.8064836770397601E-2</v>
-      </c>
-      <c r="I3">
-        <v>5.7186013768264099E-2</v>
-      </c>
-      <c r="J3">
-        <v>8.7197703707278598E-2</v>
-      </c>
-      <c r="K3">
-        <v>-0.13076106133601001</v>
-      </c>
-      <c r="L3">
-        <v>0.34148166563174398</v>
-      </c>
-      <c r="M3">
-        <v>0.47224272696775399</v>
-      </c>
-      <c r="N3">
-        <v>0.58119781062202902</v>
-      </c>
-      <c r="O3">
-        <v>0.221544658711429</v>
-      </c>
-      <c r="P3">
-        <v>1.2550270024660699E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1500</v>
-      </c>
-      <c r="F4">
-        <v>3.5552886122222301E-2</v>
-      </c>
-      <c r="G4">
-        <v>4.0148244712954403E-2</v>
-      </c>
-      <c r="H4">
-        <v>3.4194814497647101E-2</v>
-      </c>
-      <c r="I4">
-        <v>3.5246186175857501E-2</v>
-      </c>
-      <c r="J4">
-        <v>3.9717574412858503E-2</v>
-      </c>
-      <c r="K4">
-        <v>-0.123488094704773</v>
-      </c>
-      <c r="L4">
-        <v>0.16451603571780299</v>
-      </c>
-      <c r="M4">
-        <v>0.288004130422577</v>
-      </c>
-      <c r="N4">
-        <v>4.7369488451365502E-2</v>
-      </c>
-      <c r="O4">
-        <v>0.143257225626166</v>
-      </c>
-      <c r="P4">
-        <v>1.03662322101821E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>62</v>
-      </c>
-      <c r="F5">
-        <v>2.98063847473586E-2</v>
-      </c>
-      <c r="G5">
-        <v>2.5442282101289099E-2</v>
-      </c>
-      <c r="H5">
-        <v>3.04219805491023E-2</v>
-      </c>
-      <c r="I5">
-        <v>3.0665197609721501E-2</v>
-      </c>
-      <c r="J5">
-        <v>1.9737504970083902E-2</v>
-      </c>
-      <c r="K5">
-        <v>-4.1467161477593502E-2</v>
-      </c>
-      <c r="L5">
-        <v>8.8435952674173299E-2</v>
-      </c>
-      <c r="M5">
-        <v>0.129903114151766</v>
-      </c>
-      <c r="N5">
-        <v>-0.32058521689709202</v>
-      </c>
-      <c r="O5">
-        <v>0.27805982513156502</v>
-      </c>
-      <c r="P5">
-        <v>3.23117305803839E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1500</v>
-      </c>
-      <c r="F6">
-        <v>3.09034449294909E-2</v>
-      </c>
-      <c r="G6">
-        <v>2.1362621177804301E-2</v>
-      </c>
-      <c r="H6">
-        <v>3.3012378959294202E-2</v>
-      </c>
-      <c r="I6">
-        <v>3.2355747246079897E-2</v>
-      </c>
-      <c r="J6">
-        <v>1.8432211074052698E-2</v>
-      </c>
-      <c r="K6">
-        <v>-5.1403517682694098E-2</v>
-      </c>
-      <c r="L6">
-        <v>8.4344658680667497E-2</v>
-      </c>
-      <c r="M6">
-        <v>0.13574817636336101</v>
-      </c>
-      <c r="N6">
-        <v>-0.68642058074856505</v>
-      </c>
-      <c r="O6">
-        <v>0.76248592777908497</v>
-      </c>
-      <c r="P6" s="23">
-        <v>5.5158050701982703E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>62</v>
-      </c>
-      <c r="F7">
-        <v>0.103610955379368</v>
-      </c>
-      <c r="G7">
-        <v>0.15671132168063601</v>
-      </c>
-      <c r="H7">
-        <v>0.12681852649535</v>
-      </c>
-      <c r="I7">
-        <v>0.110780128453138</v>
-      </c>
-      <c r="J7">
-        <v>0.14967329512983399</v>
-      </c>
-      <c r="K7">
-        <v>-0.304004515060952</v>
-      </c>
-      <c r="L7">
-        <v>0.47735564947318498</v>
-      </c>
-      <c r="M7">
-        <v>0.78136016453413804</v>
-      </c>
-      <c r="N7">
-        <v>-0.38427129777646002</v>
-      </c>
-      <c r="O7">
-        <v>2.5557936764393201E-2</v>
-      </c>
-      <c r="P7">
-        <v>1.9902357755808401E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1500</v>
-      </c>
-      <c r="F8">
-        <v>0.107097152997913</v>
-      </c>
-      <c r="G8">
-        <v>0.16876749833910001</v>
-      </c>
-      <c r="H8">
-        <v>0.10694264976382201</v>
-      </c>
-      <c r="I8">
-        <v>0.10890629785990499</v>
-      </c>
-      <c r="J8">
-        <v>0.16081901091225301</v>
-      </c>
-      <c r="K8">
-        <v>-0.51257958073309695</v>
-      </c>
-      <c r="L8">
-        <v>0.76889643336060598</v>
-      </c>
-      <c r="M8">
-        <v>1.2814760140937</v>
-      </c>
-      <c r="N8">
-        <v>-0.120652222022161</v>
-      </c>
-      <c r="O8">
-        <v>0.49580980674382502</v>
-      </c>
-      <c r="P8">
-        <v>4.3575580696561603E-3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>